<commit_message>
Update automatico via Actualizar 05-13-2020 22-01-26
</commit_message>
<xml_diff>
--- a/datacovidhn/Indicadores_Economicos.xlsx
+++ b/datacovidhn/Indicadores_Economicos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{26D126A4-2618-4CE8-A553-B07016679878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{59887115-B717-4A92-B187-54654452F16A}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{26D126A4-2618-4CE8-A553-B07016679878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{441C0BD4-C165-4CFD-930C-C7F8CC392C04}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{15EE1032-C429-4F63-A686-A962E191E36E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -69,6 +69,42 @@
   </si>
   <si>
     <t>https://www.fxempire.es/markets/coffee/overview</t>
+  </si>
+  <si>
+    <t>Dólares Acumulados desde Enero</t>
+  </si>
+  <si>
+    <t>Promedio Diario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">632.1 millones </t>
+  </si>
+  <si>
+    <t>14.3 millones</t>
+  </si>
+  <si>
+    <t>https://www.elpais.hn/tag/remesas/</t>
+  </si>
+  <si>
+    <t>978.8 millones</t>
+  </si>
+  <si>
+    <t>15 millones</t>
+  </si>
+  <si>
+    <t>1,087.4 millones</t>
+  </si>
+  <si>
+    <t>1,187 millones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,457.2 millones </t>
+  </si>
+  <si>
+    <t>1,595.3 millones</t>
+  </si>
+  <si>
+    <t>https://proceso.hn/actualidad/7-actualidad/crece-en-10-envio-de-remesas-a-honduras-en-primer-cuatrimestre-de-2019.html</t>
   </si>
 </sst>
 </file>
@@ -158,6 +194,19 @@
     <tableColumn id="7" xr3:uid="{AB61B0F2-B71B-4FB9-8F57-8BC619A7A2B3}" name="Combustible Diesel"/>
     <tableColumn id="8" xr3:uid="{E5F57D57-825C-4007-95C9-37FF261EF551}" name="Combustible Kerosen"/>
     <tableColumn id="11" xr3:uid="{D6ADE51F-DFBE-4B2C-8B0F-5E30B0AAD1F7}" name="Café (KC) dólares/quintal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4EC15501-C300-452C-B8BC-77418C0BE5B5}" name="Tabla2" displayName="Tabla2" ref="B13:E19" totalsRowShown="0">
+  <autoFilter ref="B13:E19" xr:uid="{8DEC168B-BFE4-4E57-8F86-6C79E5B7D24D}"/>
+  <tableColumns count="4">
+    <tableColumn id="4" xr3:uid="{8B592DB8-5BE9-4754-8077-A9E8E2B847B7}" name="ID"/>
+    <tableColumn id="1" xr3:uid="{231095A9-0186-41E0-961F-D5BE7C613626}" name="Fecha"/>
+    <tableColumn id="2" xr3:uid="{FFF90E98-F696-4B63-80DA-D34D745FDE37}" name="Dólares Acumulados desde Enero"/>
+    <tableColumn id="3" xr3:uid="{4E5B462E-FD9E-4267-A04C-91505455A965}" name="Promedio Diario"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -460,15 +509,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CDD092D-D63B-44BE-89EB-E9F414DEC0DC}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="2" width="12" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
@@ -567,6 +617,35 @@
       </c>
       <c r="J3" s="2"/>
     </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43964</v>
+      </c>
+      <c r="C4">
+        <v>24.833100000000002</v>
+      </c>
+      <c r="D4" s="3">
+        <v>26.9389</v>
+      </c>
+      <c r="E4">
+        <v>68.430000000000007</v>
+      </c>
+      <c r="F4">
+        <v>61.47</v>
+      </c>
+      <c r="G4">
+        <v>54.54</v>
+      </c>
+      <c r="H4">
+        <v>32.1</v>
+      </c>
+      <c r="I4">
+        <v>105.35</v>
+      </c>
+    </row>
     <row r="7" spans="1:11">
       <c r="K7" s="2" t="s">
         <v>9</v>
@@ -582,17 +661,113 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:11" ht="15">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43874</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43895</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43902</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="15">
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="15">
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43944</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="15">
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>43946</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="15"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K8" r:id="rId1" xr:uid="{7D2A1CC9-CD5D-4FCA-8B43-A8B013D6A2FA}"/>
     <hyperlink ref="K7" r:id="rId2" xr:uid="{A344285A-BDA6-413F-9D6B-19C88FE3882A}"/>
     <hyperlink ref="K9" r:id="rId3" xr:uid="{C0F1FEDD-255D-4B46-A271-E4978045A940}"/>
+    <hyperlink ref="F14" r:id="rId4" xr:uid="{EDDC898E-9601-4ADA-94D4-456ACDD8F68B}"/>
+    <hyperlink ref="F19" r:id="rId5" xr:uid="{16C73260-CA62-4BCF-97B6-BD31B12C75C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
-  <tableParts count="1">
-    <tablePart r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <tableParts count="2">
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 05-14-2020 22-04-56
</commit_message>
<xml_diff>
--- a/datacovidhn/Indicadores_Economicos.xlsx
+++ b/datacovidhn/Indicadores_Economicos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{26D126A4-2618-4CE8-A553-B07016679878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE7FAC33-DC44-4D2D-8A6D-30D9984B82E2}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{26D126A4-2618-4CE8-A553-B07016679878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F42A0E73-CA75-4B56-86E6-7D82CBE96ECF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{15EE1032-C429-4F63-A686-A962E191E36E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -62,6 +62,9 @@
     <t>Café (KC) dólares/quintal</t>
   </si>
   <si>
+    <t>z</t>
+  </si>
+  <si>
     <t>https://www.bch.hn/index.php</t>
   </si>
   <si>
@@ -69,42 +72,6 @@
   </si>
   <si>
     <t>https://www.fxempire.es/markets/coffee/overview</t>
-  </si>
-  <si>
-    <t>Dólares Acumulados desde Enero</t>
-  </si>
-  <si>
-    <t>Promedio Diario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">632.1 millones </t>
-  </si>
-  <si>
-    <t>14.3 millones</t>
-  </si>
-  <si>
-    <t>https://www.elpais.hn/tag/remesas/</t>
-  </si>
-  <si>
-    <t>978.8 millones</t>
-  </si>
-  <si>
-    <t>15 millones</t>
-  </si>
-  <si>
-    <t>1,087.4 millones</t>
-  </si>
-  <si>
-    <t>1,187 millones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,457.2 millones </t>
-  </si>
-  <si>
-    <t>1,595.3 millones</t>
-  </si>
-  <si>
-    <t>https://proceso.hn/actualidad/7-actualidad/crece-en-10-envio-de-remesas-a-honduras-en-primer-cuatrimestre-de-2019.html</t>
   </si>
 </sst>
 </file>
@@ -194,19 +161,6 @@
     <tableColumn id="7" xr3:uid="{AB61B0F2-B71B-4FB9-8F57-8BC619A7A2B3}" name="Combustible Diesel"/>
     <tableColumn id="8" xr3:uid="{E5F57D57-825C-4007-95C9-37FF261EF551}" name="Combustible Kerosen"/>
     <tableColumn id="11" xr3:uid="{D6ADE51F-DFBE-4B2C-8B0F-5E30B0AAD1F7}" name="Café (KC) dólares/quintal"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4EC15501-C300-452C-B8BC-77418C0BE5B5}" name="Tabla2" displayName="Tabla2" ref="B13:E19" totalsRowShown="0">
-  <autoFilter ref="B13:E19" xr:uid="{8DEC168B-BFE4-4E57-8F86-6C79E5B7D24D}"/>
-  <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{8B592DB8-5BE9-4754-8077-A9E8E2B847B7}" name="ID"/>
-    <tableColumn id="1" xr3:uid="{231095A9-0186-41E0-961F-D5BE7C613626}" name="Fecha"/>
-    <tableColumn id="2" xr3:uid="{FFF90E98-F696-4B63-80DA-D34D745FDE37}" name="Dólares Acumulados desde Enero"/>
-    <tableColumn id="3" xr3:uid="{4E5B462E-FD9E-4267-A04C-91505455A965}" name="Promedio Diario"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -511,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CDD092D-D63B-44BE-89EB-E9F414DEC0DC}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:H5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B20" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -676,127 +630,55 @@
       </c>
     </row>
     <row r="7" spans="1:11">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
       <c r="K7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="K8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15">
       <c r="K9" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15">
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    </row>
+    <row r="13" spans="1:11" ht="15"/>
     <row r="14" spans="1:11" ht="15">
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>43874</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s">
-        <v>16</v>
-      </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15">
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>43895</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
-      </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="15">
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1">
-        <v>43902</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="15">
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1">
-        <v>43913</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="15">
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1">
-        <v>43944</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="15">
-      <c r="B19">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1">
-        <v>43946</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="15"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:6" ht="15">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="3:6" ht="15">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="3:6" ht="15">
+      <c r="C19" s="1"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="3:6" ht="15"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K8" r:id="rId1" xr:uid="{7D2A1CC9-CD5D-4FCA-8B43-A8B013D6A2FA}"/>
     <hyperlink ref="K7" r:id="rId2" xr:uid="{A344285A-BDA6-413F-9D6B-19C88FE3882A}"/>
     <hyperlink ref="K9" r:id="rId3" xr:uid="{C0F1FEDD-255D-4B46-A271-E4978045A940}"/>
-    <hyperlink ref="F14" r:id="rId4" xr:uid="{EDDC898E-9601-4ADA-94D4-456ACDD8F68B}"/>
-    <hyperlink ref="F19" r:id="rId5" xr:uid="{16C73260-CA62-4BCF-97B6-BD31B12C75C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
-  <tableParts count="2">
-    <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>